<commit_message>
Using median instead of mean
</commit_message>
<xml_diff>
--- a/testes/CS/J5_Log_excel.xlsx
+++ b/testes/CS/J5_Log_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACEW\Documents\Android\androidconcurrency\testes\CS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EA3275-992C-4FCE-94C2-245F983D5974}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52116059-E521-438E-9BDC-D9ABAC154746}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -599,21 +599,7 @@
     <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -940,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="V67" sqref="V67"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M58" sqref="M58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2432,70 +2418,70 @@
         <v>8</v>
       </c>
       <c r="C36">
-        <f>AVERAGE(C6:C35)</f>
-        <v>288.7</v>
+        <f>MEDIAN(C6:C35)</f>
+        <v>271.5</v>
       </c>
       <c r="D36">
-        <f t="shared" ref="D36:G36" si="0">AVERAGE(D6:D35)</f>
-        <v>281.06666666666666</v>
+        <f t="shared" ref="D36:G36" si="0">MEDIAN(D6:D35)</f>
+        <v>275.5</v>
       </c>
       <c r="E36">
         <f t="shared" si="0"/>
-        <v>413.73333333333335</v>
+        <v>419</v>
       </c>
       <c r="F36">
         <f t="shared" si="0"/>
-        <v>372.2</v>
+        <v>363</v>
       </c>
       <c r="G36">
         <f t="shared" si="0"/>
-        <v>384.33333333333331</v>
+        <v>382</v>
       </c>
       <c r="J36" t="s">
         <v>8</v>
       </c>
       <c r="K36">
-        <f>AVERAGE(K6:K35)</f>
-        <v>255.66666666666666</v>
+        <f>MEDIAN(K6:K35)</f>
+        <v>251.5</v>
       </c>
       <c r="L36">
-        <f t="shared" ref="L36" si="1">AVERAGE(L6:L35)</f>
-        <v>203.33333333333334</v>
+        <f t="shared" ref="L36:O36" si="1">MEDIAN(L6:L35)</f>
+        <v>199</v>
       </c>
       <c r="M36">
-        <f t="shared" ref="M36" si="2">AVERAGE(M6:M35)</f>
-        <v>291.96666666666664</v>
+        <f t="shared" si="1"/>
+        <v>284</v>
       </c>
       <c r="N36">
-        <f t="shared" ref="N36" si="3">AVERAGE(N6:N35)</f>
-        <v>243.9</v>
+        <f t="shared" si="1"/>
+        <v>234</v>
       </c>
       <c r="O36">
-        <f t="shared" ref="O36" si="4">AVERAGE(O6:O35)</f>
-        <v>359.43333333333334</v>
+        <f t="shared" si="1"/>
+        <v>368.5</v>
       </c>
       <c r="R36" t="s">
         <v>8</v>
       </c>
       <c r="S36">
-        <f>AVERAGE(S6:S35)</f>
-        <v>838.9666666666667</v>
+        <f>MEDIAN(S6:S35)</f>
+        <v>761.5</v>
       </c>
       <c r="T36">
-        <f t="shared" ref="T36" si="5">AVERAGE(T6:T35)</f>
-        <v>204.16666666666666</v>
+        <f t="shared" ref="T36:W36" si="2">MEDIAN(T6:T35)</f>
+        <v>201</v>
       </c>
       <c r="U36">
-        <f t="shared" ref="U36" si="6">AVERAGE(U6:U35)</f>
-        <v>305.2</v>
+        <f t="shared" si="2"/>
+        <v>307</v>
       </c>
       <c r="V36">
-        <f t="shared" ref="V36" si="7">AVERAGE(V6:V35)</f>
-        <v>248.03333333333333</v>
+        <f t="shared" si="2"/>
+        <v>251</v>
       </c>
       <c r="W36">
-        <f t="shared" ref="W36" si="8">AVERAGE(W6:W35)</f>
-        <v>566.5</v>
+        <f t="shared" si="2"/>
+        <v>544.5</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
@@ -2507,19 +2493,19 @@
         <v>30.806666666666654</v>
       </c>
       <c r="D37">
-        <f t="shared" ref="D37:G37" si="9">AVEDEV(D6:D35)</f>
+        <f t="shared" ref="D37:G37" si="3">AVEDEV(D6:D35)</f>
         <v>12.217777777777776</v>
       </c>
       <c r="E37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>37.417777777777779</v>
       </c>
       <c r="F37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>33.773333333333341</v>
       </c>
       <c r="G37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>33.955555555555549</v>
       </c>
       <c r="J37" t="s">
@@ -2530,19 +2516,19 @@
         <v>10.355555555555551</v>
       </c>
       <c r="L37">
-        <f t="shared" ref="L37:O37" si="10">AVEDEV(L6:L35)</f>
+        <f t="shared" ref="L37:O37" si="4">AVEDEV(L6:L35)</f>
         <v>8.7333333333333378</v>
       </c>
       <c r="M37">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>19.817777777777771</v>
       </c>
       <c r="N37">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>25.193333333333328</v>
       </c>
       <c r="O37">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>35.204444444444448</v>
       </c>
       <c r="R37" t="s">
@@ -2553,19 +2539,19 @@
         <v>132.28222222222223</v>
       </c>
       <c r="T37">
-        <f t="shared" ref="T37:W37" si="11">AVEDEV(T6:T35)</f>
+        <f t="shared" ref="T37:W37" si="5">AVEDEV(T6:T35)</f>
         <v>6.1666666666666625</v>
       </c>
       <c r="U37">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>9.2533333333333339</v>
       </c>
       <c r="V37">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>19.831111111111117</v>
       </c>
       <c r="W37">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>58.8</v>
       </c>
     </row>
@@ -3266,7 +3252,7 @@
       <c r="L58">
         <v>804</v>
       </c>
-      <c r="M58">
+      <c r="M58" s="1">
         <v>831</v>
       </c>
       <c r="N58">
@@ -4048,47 +4034,47 @@
         <v>8</v>
       </c>
       <c r="C75">
-        <f>AVERAGE(C45:C74)</f>
-        <v>1063.4333333333334</v>
+        <f>MEDIAN(C45:C74)</f>
+        <v>1050</v>
       </c>
       <c r="D75">
-        <f t="shared" ref="D75:G75" si="12">AVERAGE(D45:D74)</f>
-        <v>1130.8666666666666</v>
+        <f t="shared" ref="D75:G75" si="6">MEDIAN(D45:D74)</f>
+        <v>1098</v>
       </c>
       <c r="E75">
-        <f t="shared" si="12"/>
-        <v>1175.8</v>
+        <f t="shared" si="6"/>
+        <v>1151</v>
       </c>
       <c r="F75">
-        <f t="shared" si="12"/>
-        <v>1283.2</v>
+        <f t="shared" si="6"/>
+        <v>1253</v>
       </c>
       <c r="G75">
-        <f t="shared" si="12"/>
-        <v>1732.7666666666667</v>
+        <f t="shared" si="6"/>
+        <v>1751.5</v>
       </c>
       <c r="J75" t="s">
         <v>8</v>
       </c>
       <c r="K75">
-        <f>AVERAGE(K45:K74)</f>
-        <v>837.9666666666667</v>
+        <f>MEDIAN(K45:K74)</f>
+        <v>830.5</v>
       </c>
       <c r="L75">
-        <f t="shared" ref="L75:O75" si="13">AVERAGE(L45:L74)</f>
-        <v>809.86666666666667</v>
+        <f t="shared" ref="L75:O75" si="7">MEDIAN(L45:L74)</f>
+        <v>799</v>
       </c>
       <c r="M75">
-        <f t="shared" si="13"/>
-        <v>868.76666666666665</v>
+        <f t="shared" si="7"/>
+        <v>852</v>
       </c>
       <c r="N75">
-        <f t="shared" si="13"/>
-        <v>816.4666666666667</v>
+        <f t="shared" si="7"/>
+        <v>813.5</v>
       </c>
       <c r="O75">
-        <f t="shared" si="13"/>
-        <v>1537.9</v>
+        <f t="shared" si="7"/>
+        <v>1500</v>
       </c>
       <c r="R75" t="s">
         <v>8</v>
@@ -4098,19 +4084,19 @@
         <v>1649.1333333333334</v>
       </c>
       <c r="T75">
-        <f t="shared" ref="T75:W75" si="14">AVERAGE(T45:T74)</f>
+        <f t="shared" ref="T75:W75" si="8">AVERAGE(T45:T74)</f>
         <v>807.56666666666672</v>
       </c>
       <c r="U75">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>931.56666666666672</v>
       </c>
       <c r="V75">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>822.5333333333333</v>
       </c>
       <c r="W75">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>1743.5333333333333</v>
       </c>
     </row>
@@ -4123,19 +4109,19 @@
         <v>26.79777777777781</v>
       </c>
       <c r="D76">
-        <f t="shared" ref="D76:G76" si="15">AVEDEV(D45:D74)</f>
+        <f t="shared" ref="D76:G76" si="9">AVEDEV(D45:D74)</f>
         <v>55.035555555555476</v>
       </c>
       <c r="E76">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>45.719999999999963</v>
       </c>
       <c r="F76">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>71.44</v>
       </c>
       <c r="G76">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>39.968888888888905</v>
       </c>
       <c r="J76" t="s">
@@ -4146,19 +4132,19 @@
         <v>19.422222222222231</v>
       </c>
       <c r="L76">
-        <f t="shared" ref="L76:O76" si="16">AVEDEV(L45:L74)</f>
+        <f t="shared" ref="L76:O76" si="10">AVEDEV(L45:L74)</f>
         <v>21.204444444444448</v>
       </c>
       <c r="M76">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>32.042222222222215</v>
       </c>
       <c r="N76">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>14.960000000000006</v>
       </c>
       <c r="O76">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>58.646666666666718</v>
       </c>
       <c r="R76" t="s">
@@ -4169,30 +4155,30 @@
         <v>191.20888888888894</v>
       </c>
       <c r="T76">
-        <f t="shared" ref="T76:W76" si="17">AVEDEV(T45:T74)</f>
+        <f t="shared" ref="T76:W76" si="11">AVEDEV(T45:T74)</f>
         <v>20.393333333333356</v>
       </c>
       <c r="U76">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>44.175555555555562</v>
       </c>
       <c r="V76">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>19.035555555555554</v>
       </c>
       <c r="W76">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>33.573333333333331</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C6:G35 K6:O35 S6:W35 AA6:AE35 AI6:AM35">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>OR(C6&gt;C$36+C$37*2,C6&lt;C$36-2*C$37)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:G74 K45:O74 S45:W74">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>OR(C45&gt;C$75+C$76*2,C45&lt;C$75-2*C$76)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Substituted Average by Median on excel files
</commit_message>
<xml_diff>
--- a/testes/CS/J5_Log_excel.xlsx
+++ b/testes/CS/J5_Log_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACEW\Documents\Android\androidconcurrency\testes\CS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52116059-E521-438E-9BDC-D9ABAC154746}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A65D9E9-7B90-460C-873E-1F006643E3B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,13 +53,13 @@
     <t>Threads with barriers</t>
   </si>
   <si>
-    <t>Average</t>
-  </si>
-  <si>
     <t>Deviation</t>
   </si>
   <si>
     <t>16 Tasks</t>
+  </si>
+  <si>
+    <t>Median</t>
   </si>
 </sst>
 </file>
@@ -556,48 +556,48 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bom" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Célula de Verificação" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Célula Vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Ênfase1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Ênfase2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Ênfase3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Ênfase4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Ênfase5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Ênfase6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Neutro" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Ruim" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de Aviso" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto Explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -628,7 +628,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -926,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M58" sqref="M58"/>
+    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,7 +950,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R4" t="s">
         <v>2</v>
@@ -2415,7 +2415,7 @@
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C36">
         <f>MEDIAN(C6:C35)</f>
@@ -2438,7 +2438,7 @@
         <v>382</v>
       </c>
       <c r="J36" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K36">
         <f>MEDIAN(K6:K35)</f>
@@ -2461,7 +2461,7 @@
         <v>368.5</v>
       </c>
       <c r="R36" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="S36">
         <f>MEDIAN(S6:S35)</f>
@@ -2486,7 +2486,7 @@
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C37">
         <f>AVEDEV(C6:C35)</f>
@@ -2509,7 +2509,7 @@
         <v>33.955555555555549</v>
       </c>
       <c r="J37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K37">
         <f>AVEDEV(K6:K35)</f>
@@ -2532,7 +2532,7 @@
         <v>35.204444444444448</v>
       </c>
       <c r="R37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S37">
         <f>AVEDEV(S6:S35)</f>
@@ -2565,7 +2565,7 @@
         <v>1</v>
       </c>
       <c r="J43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R43" t="s">
         <v>2</v>
@@ -4031,7 +4031,7 @@
     </row>
     <row r="75" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C75">
         <f>MEDIAN(C45:C74)</f>
@@ -4054,7 +4054,7 @@
         <v>1751.5</v>
       </c>
       <c r="J75" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K75">
         <f>MEDIAN(K45:K74)</f>
@@ -4077,7 +4077,7 @@
         <v>1500</v>
       </c>
       <c r="R75" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="S75">
         <f>AVERAGE(S45:S74)</f>
@@ -4102,7 +4102,7 @@
     </row>
     <row r="76" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C76">
         <f>AVEDEV(C45:C74)</f>
@@ -4125,7 +4125,7 @@
         <v>39.968888888888905</v>
       </c>
       <c r="J76" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K76">
         <f>AVEDEV(K45:K74)</f>
@@ -4148,7 +4148,7 @@
         <v>58.646666666666718</v>
       </c>
       <c r="R76" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S76">
         <f>AVEDEV(S45:S74)</f>

</xml_diff>

<commit_message>
Added graphics to CS excel file
</commit_message>
<xml_diff>
--- a/testes/CS/J5_Log_excel.xlsx
+++ b/testes/CS/J5_Log_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACEW\Documents\Android\androidconcurrency\testes\CS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A65D9E9-7B90-460C-873E-1F006643E3B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05E4A83-16AD-4DFD-AC9C-699F122E38BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="14">
   <si>
     <t>Concurrent sum</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>Median</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Thread Pool</t>
+  </si>
+  <si>
+    <t>Threads com barreiras</t>
   </si>
 </sst>
 </file>
@@ -551,9 +560,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -599,7 +609,14 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -625,6 +642,2774 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Tempo</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> de execução com 262144 números</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>J5_Log_agreggated!$AB$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Threads</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$AC$5:$AE$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$AC$6:$AE$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>271.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>251.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>761.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-427C-488B-9C87-77EA0F00C6D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>J5_Log_agreggated!$AB$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Thread Pool</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$AC$5:$AE$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$AC$7:$AE$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>275.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-427C-488B-9C87-77EA0F00C6D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>J5_Log_agreggated!$AB$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HaMeR framework</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$AC$5:$AE$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$AC$8:$AE$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>307</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-427C-488B-9C87-77EA0F00C6D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>J5_Log_agreggated!$AB$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Kotlin coroutines</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$AC$5:$AE$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$AC$9:$AE$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>363</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>251</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-427C-488B-9C87-77EA0F00C6D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>J5_Log_agreggated!$AB$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Threads com barreiras</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$AC$5:$AE$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$AC$10:$AE$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>382</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>368.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>544.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-427C-488B-9C87-77EA0F00C6D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="397187816"/>
+        <c:axId val="397186504"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="397187816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Tarefas</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="397186504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="397186504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Tempo</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-BR" baseline="0"/>
+                  <a:t> (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="397187816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Tempo</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> de execução com 1048576 números</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>J5_Log_agreggated!$AA$57</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Threads</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$AB$56:$AD$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$AB$57:$AD$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>830.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1533.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EB7F-449D-8A1D-94FD02AB7E1C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>J5_Log_agreggated!$AA$58</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Thread Pool</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$AB$56:$AD$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$AB$58:$AD$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1098</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>799</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EB7F-449D-8A1D-94FD02AB7E1C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>J5_Log_agreggated!$AA$59</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HaMeR framework</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$AB$56:$AD$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$AB$59:$AD$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1151</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>852</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>914.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EB7F-449D-8A1D-94FD02AB7E1C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>J5_Log_agreggated!$AA$60</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Kotlin coroutines</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$AB$56:$AD$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$AB$60:$AD$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1253</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>813.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>818</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-EB7F-449D-8A1D-94FD02AB7E1C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>J5_Log_agreggated!$AA$61</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Threads com barreiras</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$AB$56:$AD$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>J5_Log_agreggated!$AB$61:$AD$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1751.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1733.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-EB7F-449D-8A1D-94FD02AB7E1C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="397187816"/>
+        <c:axId val="397186504"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="397187816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Tarefas</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="397186504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="397186504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Tempo</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-BR" baseline="0"/>
+                  <a:t> (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="397187816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>865908</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>122956</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>484909</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>17318</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5F73622-CE1F-4078-8EDF-34AF3979B06F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>900545</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>519546</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>69273</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E30FCA0-4C9D-44B1-B685-5589C9DB7FFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -924,10 +3709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W76"/>
+  <dimension ref="A1:AI76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="S50" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AA56" sqref="AA56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,17 +3720,17 @@
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>262144</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -956,7 +3741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>3</v>
       </c>
@@ -1002,8 +3787,17 @@
       <c r="W5" t="s">
         <v>7</v>
       </c>
+      <c r="AC5">
+        <v>1</v>
+      </c>
+      <c r="AD5">
+        <v>16</v>
+      </c>
+      <c r="AE5">
+        <v>256</v>
+      </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>270</v>
       </c>
@@ -1049,8 +3843,20 @@
       <c r="W6">
         <v>552</v>
       </c>
+      <c r="AB6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC6">
+        <v>271.5</v>
+      </c>
+      <c r="AD6">
+        <v>251.5</v>
+      </c>
+      <c r="AE6">
+        <v>761.5</v>
+      </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>277</v>
       </c>
@@ -1096,8 +3902,20 @@
       <c r="W7">
         <v>574</v>
       </c>
+      <c r="AB7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC7">
+        <v>275.5</v>
+      </c>
+      <c r="AD7">
+        <v>199</v>
+      </c>
+      <c r="AE7">
+        <v>201</v>
+      </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>273</v>
       </c>
@@ -1143,8 +3961,20 @@
       <c r="W8">
         <v>465</v>
       </c>
+      <c r="AB8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC8">
+        <v>419</v>
+      </c>
+      <c r="AD8">
+        <v>284</v>
+      </c>
+      <c r="AE8">
+        <v>307</v>
+      </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>259</v>
       </c>
@@ -1190,8 +4020,20 @@
       <c r="W9">
         <v>547</v>
       </c>
+      <c r="AB9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC9">
+        <v>363</v>
+      </c>
+      <c r="AD9">
+        <v>234</v>
+      </c>
+      <c r="AE9">
+        <v>251</v>
+      </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>261</v>
       </c>
@@ -1237,8 +4079,20 @@
       <c r="W10">
         <v>491</v>
       </c>
+      <c r="AB10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC10">
+        <v>382</v>
+      </c>
+      <c r="AD10">
+        <v>368.5</v>
+      </c>
+      <c r="AE10">
+        <v>544.5</v>
+      </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>265</v>
       </c>
@@ -1285,7 +4139,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>267</v>
       </c>
@@ -1332,7 +4186,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>273</v>
       </c>
@@ -1379,7 +4233,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>261</v>
       </c>
@@ -1426,7 +4280,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>258</v>
       </c>
@@ -1473,7 +4327,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>264</v>
       </c>
@@ -1520,7 +4374,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="17" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>314</v>
       </c>
@@ -1567,7 +4421,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="18" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>277</v>
       </c>
@@ -1614,7 +4468,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="19" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>259</v>
       </c>
@@ -1661,7 +4515,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="20" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>273</v>
       </c>
@@ -1708,7 +4562,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="21" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>270</v>
       </c>
@@ -1755,7 +4609,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="22" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>283</v>
       </c>
@@ -1802,7 +4656,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="23" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>283</v>
       </c>
@@ -1849,7 +4703,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="24" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>269</v>
       </c>
@@ -1896,7 +4750,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="25" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>257</v>
       </c>
@@ -1943,7 +4797,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="26" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>269</v>
       </c>
@@ -1990,7 +4844,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="27" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>279</v>
       </c>
@@ -2037,7 +4891,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="28" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>289</v>
       </c>
@@ -2084,7 +4938,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="29" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>266</v>
       </c>
@@ -2131,7 +4985,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="30" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C30">
         <v>265</v>
       </c>
@@ -2178,7 +5032,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="31" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>296</v>
       </c>
@@ -2225,7 +5079,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="32" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>470</v>
       </c>
@@ -2270,6 +5124,9 @@
       </c>
       <c r="W32">
         <v>558</v>
+      </c>
+      <c r="AI32" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
@@ -2806,7 +5663,7 @@
         <v>1758</v>
       </c>
     </row>
-    <row r="49" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C49">
         <v>1042</v>
       </c>
@@ -2853,7 +5710,7 @@
         <v>1717</v>
       </c>
     </row>
-    <row r="50" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C50">
         <v>1039</v>
       </c>
@@ -2900,7 +5757,7 @@
         <v>1701</v>
       </c>
     </row>
-    <row r="51" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C51">
         <v>1081</v>
       </c>
@@ -2947,7 +5804,7 @@
         <v>1764</v>
       </c>
     </row>
-    <row r="52" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C52">
         <v>1044</v>
       </c>
@@ -2995,7 +5852,7 @@
         <v>1777</v>
       </c>
     </row>
-    <row r="53" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C53">
         <v>1040</v>
       </c>
@@ -3042,7 +5899,7 @@
         <v>1735</v>
       </c>
     </row>
-    <row r="54" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C54">
         <v>1062</v>
       </c>
@@ -3089,7 +5946,7 @@
         <v>1706</v>
       </c>
     </row>
-    <row r="55" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C55">
         <v>1080</v>
       </c>
@@ -3136,7 +5993,7 @@
         <v>1754</v>
       </c>
     </row>
-    <row r="56" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C56">
         <v>1032</v>
       </c>
@@ -3182,8 +6039,17 @@
       <c r="W56">
         <v>1733</v>
       </c>
+      <c r="AB56">
+        <v>1</v>
+      </c>
+      <c r="AC56">
+        <v>16</v>
+      </c>
+      <c r="AD56">
+        <v>256</v>
+      </c>
     </row>
-    <row r="57" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C57">
         <v>1052</v>
       </c>
@@ -3229,8 +6095,20 @@
       <c r="W57">
         <v>1687</v>
       </c>
+      <c r="AA57" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB57">
+        <v>1050</v>
+      </c>
+      <c r="AC57">
+        <v>830.5</v>
+      </c>
+      <c r="AD57">
+        <v>1533.5</v>
+      </c>
     </row>
-    <row r="58" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C58">
         <v>1049</v>
       </c>
@@ -3276,8 +6154,20 @@
       <c r="W58">
         <v>1734</v>
       </c>
+      <c r="AA58" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB58">
+        <v>1098</v>
+      </c>
+      <c r="AC58">
+        <v>799</v>
+      </c>
+      <c r="AD58">
+        <v>800</v>
+      </c>
     </row>
-    <row r="59" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C59">
         <v>1041</v>
       </c>
@@ -3323,8 +6213,20 @@
       <c r="W59">
         <v>1703</v>
       </c>
+      <c r="AA59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB59">
+        <v>1151</v>
+      </c>
+      <c r="AC59">
+        <v>852</v>
+      </c>
+      <c r="AD59">
+        <v>914.5</v>
+      </c>
     </row>
-    <row r="60" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C60">
         <v>1070</v>
       </c>
@@ -3370,8 +6272,20 @@
       <c r="W60">
         <v>1722</v>
       </c>
+      <c r="AA60" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB60">
+        <v>1253</v>
+      </c>
+      <c r="AC60">
+        <v>813.5</v>
+      </c>
+      <c r="AD60">
+        <v>818</v>
+      </c>
     </row>
-    <row r="61" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C61">
         <v>1038</v>
       </c>
@@ -3417,8 +6331,20 @@
       <c r="W61">
         <v>1753</v>
       </c>
+      <c r="AA61" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB61">
+        <v>1751.5</v>
+      </c>
+      <c r="AC61">
+        <v>1500</v>
+      </c>
+      <c r="AD61">
+        <v>1733.5</v>
+      </c>
     </row>
-    <row r="62" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C62">
         <v>1079</v>
       </c>
@@ -3465,7 +6391,7 @@
         <v>1697</v>
       </c>
     </row>
-    <row r="63" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C63">
         <v>1062</v>
       </c>
@@ -3512,7 +6438,7 @@
         <v>1698</v>
       </c>
     </row>
-    <row r="64" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C64">
         <v>1062</v>
       </c>
@@ -4080,24 +7006,24 @@
         <v>10</v>
       </c>
       <c r="S75">
-        <f>AVERAGE(S45:S74)</f>
-        <v>1649.1333333333334</v>
+        <f>MEDIAN(S45:S74)</f>
+        <v>1533.5</v>
       </c>
       <c r="T75">
-        <f t="shared" ref="T75:W75" si="8">AVERAGE(T45:T74)</f>
-        <v>807.56666666666672</v>
+        <f t="shared" ref="T75:W75" si="8">MEDIAN(T45:T74)</f>
+        <v>800</v>
       </c>
       <c r="U75">
         <f t="shared" si="8"/>
-        <v>931.56666666666672</v>
+        <v>914.5</v>
       </c>
       <c r="V75">
         <f t="shared" si="8"/>
-        <v>822.5333333333333</v>
+        <v>818</v>
       </c>
       <c r="W75">
         <f t="shared" si="8"/>
-        <v>1743.5333333333333</v>
+        <v>1733.5</v>
       </c>
     </row>
     <row r="76" spans="2:23" x14ac:dyDescent="0.25">
@@ -4172,17 +7098,23 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C6:G35 K6:O35 S6:W35 AA6:AE35 AI6:AM35">
-    <cfRule type="expression" dxfId="1" priority="2">
+  <conditionalFormatting sqref="C6:G35 K6:O35 S6:W35 AA7:AE35 AI6:AM35 AA6">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>OR(C6&gt;C$36+C$37*2,C6&lt;C$36-2*C$37)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:G74 K45:O74 S45:W74">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>OR(C45&gt;C$75+C$76*2,C45&lt;C$75-2*C$76)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA58:AD61">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>OR(C45&gt;C$75+C$76*2,C45&lt;C$75-2*C$76)</formula>
+      <formula>OR(AA58&gt;AA$36+AA$37*2,AA58&lt;AA$36-2*AA$37)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated tables with some p-values
</commit_message>
<xml_diff>
--- a/testes/CS/J5_Log_excel.xlsx
+++ b/testes/CS/J5_Log_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACEW\Documents\Android\androidconcurrency\testes\CS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05E4A83-16AD-4DFD-AC9C-699F122E38BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8C2AA1-4F39-42AA-8416-8473E499FBC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12540" yWindow="5700" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="J5_Log_agreggated" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -3711,8 +3712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S50" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AA56" sqref="AA56"/>
+    <sheetView tabSelected="1" topLeftCell="K42" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="P73" sqref="P73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5756,6 +5757,10 @@
       <c r="W50">
         <v>1701</v>
       </c>
+      <c r="Z50">
+        <f>_xlfn.T.TEST(T45:T74,V45:V74,2,3)</f>
+        <v>2.9826430828330208E-2</v>
+      </c>
     </row>
     <row r="51" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C51">
@@ -5882,6 +5887,10 @@
       </c>
       <c r="O53">
         <v>1486</v>
+      </c>
+      <c r="Q53">
+        <f>_xlfn.T.TEST(L45:L74,N45:N74,2,3)</f>
+        <v>0.36510161225272908</v>
       </c>
       <c r="S53">
         <v>1683</v>

</xml_diff>